<commit_message>
XML End Point change
</commit_message>
<xml_diff>
--- a/target/META-INF/mule-src/devopsdemo/testScripts/GET.xlsx
+++ b/target/META-INF/mule-src/devopsdemo/testScripts/GET.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Response</t>
   </si>
@@ -30,38 +30,7 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>HTTP/1.1 200 
-Content-Length: 13
-Date: Wed, 29 May 2019 13:05:04 GMT
-Hello World..</t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 
-Content-Length: 13
-Date: Wed, 29 May 2019 13:05:32 GMT
-Hello World..</t>
-  </si>
-  <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 
-Content-Length: 13
-Date: Mon, 03 Jun 2019 07:39:18 GMT
-Hello World..</t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 
-Content-Length: 13
-Date: Mon, 10 Jun 2019 05:25:35 GMT
-Hello World..</t>
-  </si>
-  <si>
-    <t>HTTP/1.1 200 
-Content-Type: application/java; charset=windows-1252
-Content-Length: 13
-Date: Thu, 13 Jun 2019 06:14:05 GMT
-CI/CD Demo...</t>
   </si>
   <si>
     <t>HTTP/1.1 200 
@@ -75,7 +44,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,14 +389,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,26 +410,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
+    <row r="2" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>401</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>